<commit_message>
1137 + progress file
</commit_message>
<xml_diff>
--- a/leetcode_progress.xlsx
+++ b/leetcode_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies\A_Coding_Folder\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6657FDAD-D05E-42AC-A0B1-68C817094D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0E20B7-8D09-4809-9D03-F479A485C88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="95">
   <si>
     <t>Question</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -406,6 +406,14 @@
   </si>
   <si>
     <t>5min + 10min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5min + 30min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10min + 10min</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -808,7 +816,7 @@
   <dimension ref="A1:F371"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3062,60 +3070,87 @@
       <c r="B143" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C143" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D143" s="3">
         <v>44915</v>
       </c>
       <c r="F143" s="4"/>
     </row>
     <row r="144" spans="1:6">
+      <c r="A144" s="2">
+        <v>509</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D144" s="3">
+        <v>44927</v>
+      </c>
       <c r="F144" s="4"/>
     </row>
-    <row r="145" spans="6:6">
+    <row r="145" spans="1:6">
+      <c r="A145" s="2">
+        <v>1137</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D145" s="3">
+        <v>44927</v>
+      </c>
       <c r="F145" s="4"/>
     </row>
-    <row r="146" spans="6:6">
+    <row r="146" spans="1:6">
       <c r="F146" s="4"/>
     </row>
-    <row r="147" spans="6:6">
+    <row r="147" spans="1:6">
       <c r="F147" s="4"/>
     </row>
-    <row r="148" spans="6:6">
+    <row r="148" spans="1:6">
       <c r="F148" s="4"/>
     </row>
-    <row r="149" spans="6:6">
+    <row r="149" spans="1:6">
       <c r="F149" s="4"/>
     </row>
-    <row r="150" spans="6:6">
+    <row r="150" spans="1:6">
       <c r="F150" s="4"/>
     </row>
-    <row r="151" spans="6:6">
+    <row r="151" spans="1:6">
       <c r="F151" s="4"/>
     </row>
-    <row r="152" spans="6:6">
+    <row r="152" spans="1:6">
       <c r="F152" s="4"/>
     </row>
-    <row r="153" spans="6:6">
+    <row r="153" spans="1:6">
       <c r="F153" s="4"/>
     </row>
-    <row r="154" spans="6:6">
+    <row r="154" spans="1:6">
       <c r="F154" s="4"/>
     </row>
-    <row r="155" spans="6:6">
+    <row r="155" spans="1:6">
       <c r="F155" s="4"/>
     </row>
-    <row r="156" spans="6:6">
+    <row r="156" spans="1:6">
       <c r="F156" s="4"/>
     </row>
-    <row r="157" spans="6:6">
+    <row r="157" spans="1:6">
       <c r="F157" s="4"/>
     </row>
-    <row r="158" spans="6:6">
+    <row r="158" spans="1:6">
       <c r="F158" s="4"/>
     </row>
-    <row r="159" spans="6:6">
+    <row r="159" spans="1:6">
       <c r="F159" s="4"/>
     </row>
-    <row r="160" spans="6:6">
+    <row r="160" spans="1:6">
       <c r="F160" s="4"/>
     </row>
     <row r="161" spans="6:6">

</xml_diff>